<commit_message>
Add meeting dates: 3rd Monday each month, 1:00-2:30 PM
- All meetings on 3rd Monday except Feb 17 (moved from 2/16 holiday)
- Added reminder dates (2 weeks before each meeting)
- Updated all email templates with specific dates

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Downloads/All_Staff_Meeting_Coordination/04_All_Staff_Facilitator_Tracker.xlsx
+++ b/Downloads/All_Staff_Meeting_Coordination/04_All_Staff_Facilitator_Tracker.xlsx
@@ -457,7 +457,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,12 +543,12 @@
       <c r="C2" s="6" t="inlineStr"/>
       <c r="D2" s="6" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>1/19</t>
         </is>
       </c>
       <c r="E2" s="6" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>1/5</t>
         </is>
       </c>
       <c r="F2" s="6" t="inlineStr">
@@ -591,12 +591,12 @@
       <c r="C3" s="3" t="inlineStr"/>
       <c r="D3" s="3" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>2/17 (Tue)</t>
         </is>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>2/3</t>
         </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
@@ -639,12 +639,12 @@
       <c r="C4" s="2" t="inlineStr"/>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>3/16</t>
         </is>
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>2 wks before</t>
+          <t>3/2</t>
         </is>
       </c>
       <c r="F4" s="2" t="inlineStr"/>
@@ -671,12 +671,12 @@
       <c r="C5" s="3" t="inlineStr"/>
       <c r="D5" s="3" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>4/20</t>
         </is>
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>2 wks before</t>
+          <t>4/6</t>
         </is>
       </c>
       <c r="F5" s="3" t="inlineStr"/>
@@ -703,12 +703,12 @@
       <c r="C6" s="2" t="inlineStr"/>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>5/18</t>
         </is>
       </c>
       <c r="E6" s="2" t="inlineStr">
         <is>
-          <t>2 wks before</t>
+          <t>5/4</t>
         </is>
       </c>
       <c r="F6" s="2" t="inlineStr"/>
@@ -735,12 +735,12 @@
       <c r="C7" s="3" t="inlineStr"/>
       <c r="D7" s="3" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>6/15</t>
         </is>
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>2 wks before</t>
+          <t>6/1</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr"/>
@@ -767,12 +767,12 @@
       <c r="C8" s="2" t="inlineStr"/>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>7/20</t>
         </is>
       </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
-          <t>2 wks before</t>
+          <t>7/6</t>
         </is>
       </c>
       <c r="F8" s="2" t="inlineStr"/>
@@ -799,12 +799,12 @@
       <c r="C9" s="3" t="inlineStr"/>
       <c r="D9" s="3" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>8/17</t>
         </is>
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>2 wks before</t>
+          <t>8/3</t>
         </is>
       </c>
       <c r="F9" s="3" t="inlineStr"/>
@@ -835,12 +835,12 @@
       <c r="C10" s="2" t="inlineStr"/>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>9/21</t>
         </is>
       </c>
       <c r="E10" s="2" t="inlineStr">
         <is>
-          <t>2 wks before</t>
+          <t>9/7</t>
         </is>
       </c>
       <c r="F10" s="2" t="inlineStr"/>
@@ -871,12 +871,12 @@
       <c r="C11" s="3" t="inlineStr"/>
       <c r="D11" s="3" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>10/19</t>
         </is>
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>2 wks before</t>
+          <t>10/5</t>
         </is>
       </c>
       <c r="F11" s="3" t="inlineStr"/>
@@ -907,12 +907,12 @@
       <c r="C12" s="2" t="inlineStr"/>
       <c r="D12" s="2" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>11/16</t>
         </is>
       </c>
       <c r="E12" s="2" t="inlineStr">
         <is>
-          <t>2 wks before</t>
+          <t>11/2</t>
         </is>
       </c>
       <c r="F12" s="2" t="inlineStr"/>
@@ -943,12 +943,12 @@
       <c r="C13" s="3" t="inlineStr"/>
       <c r="D13" s="3" t="inlineStr">
         <is>
-          <t>TBD</t>
+          <t>12/21</t>
         </is>
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>2 wks before</t>
+          <t>12/7</t>
         </is>
       </c>
       <c r="F13" s="3" t="inlineStr"/>

</xml_diff>